<commit_message>
Se agrega la tabla de divisiones de primer, segundo, tercer y cuarto orden, tambien se ajusta el informe
</commit_message>
<xml_diff>
--- a/Parcial-Ejercicio-Regresion.xlsx
+++ b/Parcial-Ejercicio-Regresion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicaucaeduco-my.sharepoint.com/personal/juanoa_unicauca_edu_co/Documents/UNIVERSIDAD/Semestre2021.1/Analisis Numerico/Parcial-2-2021-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="509" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{23A1B721-8F99-41C1-94D5-AF7B79A9B9D9}"/>
+  <xr:revisionPtr revIDLastSave="599" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{88FEB871-F202-47FE-9FCC-5B1A14EFA38C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -64,15 +64,6 @@
     <t>x0,y0</t>
   </si>
   <si>
-    <t>Polinomio de interpolacion de primer grado</t>
-  </si>
-  <si>
-    <t>Polinomio de interpolacion de segundo grado</t>
-  </si>
-  <si>
-    <t>Polinomio de interpolacion de tercer grado</t>
-  </si>
-  <si>
     <t>2A. DIFERENCIA</t>
   </si>
   <si>
@@ -83,6 +74,60 @@
   </si>
   <si>
     <t>4A. DIFERENCIA</t>
+  </si>
+  <si>
+    <t>F(x0,x1)</t>
+  </si>
+  <si>
+    <t>F(x1,x2)</t>
+  </si>
+  <si>
+    <t>F(X2,X3)</t>
+  </si>
+  <si>
+    <t>F(X3,X4)</t>
+  </si>
+  <si>
+    <t>F(X4,X5)</t>
+  </si>
+  <si>
+    <t>F(X5,X6)</t>
+  </si>
+  <si>
+    <t>F(X0,X1,X2)</t>
+  </si>
+  <si>
+    <t>F(X1,X2,X3)</t>
+  </si>
+  <si>
+    <t>F(X2,X3,X4)</t>
+  </si>
+  <si>
+    <t>F(X3,X4,X5)</t>
+  </si>
+  <si>
+    <t>F(X4,X5,X6)</t>
+  </si>
+  <si>
+    <t>F(X0,X1,X2,X3)</t>
+  </si>
+  <si>
+    <t>F(X1,X2,X3,X4)</t>
+  </si>
+  <si>
+    <t>F(X2,X3,X4,X5)</t>
+  </si>
+  <si>
+    <t>F(X3,X4,X5,X6)</t>
+  </si>
+  <si>
+    <t>F(X0,X1,X2,X3,X4)</t>
+  </si>
+  <si>
+    <t>F(X1,X2,X3,X4,X5)</t>
+  </si>
+  <si>
+    <t>F(X2,X3,X4,X5,X6)</t>
   </si>
 </sst>
 </file>
@@ -98,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,8 +174,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -229,21 +280,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -311,9 +347,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -331,14 +364,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4408,7 +4446,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5061258A-C493-4EB4-80EF-5B534CFDB04E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4444,7 +4482,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D796AE8-23A3-4F78-A232-EA8137A4EA9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4480,7 +4518,7 @@
         <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42C01241-D5DA-44EB-A903-0EB9C91BA005}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4521,7 +4559,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1348062-B8B6-44DE-B5DA-2EAB80960EAC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4539,226 +4577,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2049" name="Object 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2049"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDF223A2-B0B1-467F-B80E-CCD295B6ECD5}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>95250</xdr:colOff>
-          <xdr:row>22</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2050" name="Object 2" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2050"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B6AC9B3-27B1-41DA-A31E-FC7D274345CE}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
-          <xdr:row>22</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>666750</xdr:colOff>
-          <xdr:row>24</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2051" name="Object 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2051"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6A27E06-CE4E-4AD4-9EE8-9724A04BC08F}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
-          <xdr:row>25</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2052" name="Object 4" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2052"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2819F892-65C2-471B-9D75-B5B8E22F1B6E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -5206,10 +5024,10 @@
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5290,10 +5108,10 @@
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5370,8 +5188,8 @@
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" s="2"/>
@@ -5411,24 +5229,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75BD078-DD7C-4543-9D69-F110EEC51D30}">
-  <dimension ref="B3:M39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75BD078-DD7C-4543-9D69-F110EEC51D30}">
+  <dimension ref="B3:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="21" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5510,232 +5330,206 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="15">
+        <f>(D5-D4)/(C5-C4)</f>
+        <v>40</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
-        <v>10</v>
-      </c>
+      <c r="B20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="15">
+        <f>(D6-D5)/(C6-C5)</f>
+        <v>-162.5</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="15">
+        <f>(C20-C19)/(C6-C4)</f>
+        <v>-2025</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="15">
+        <f t="shared" ref="C21:C24" si="0">(D7-D6)/(C7-C6)</f>
+        <v>4700.0000000000009</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="15">
+        <f>(C21-C20)/(C7-C5)</f>
+        <v>-13892.857142857147</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="15">
+        <f>(E21-E20)/(C7-C4)</f>
+        <v>-79119.047619047647</v>
+      </c>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="2:13" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="21"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="13"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="14"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="16"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="15"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="16"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="15"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="16"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="15"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="16"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="15"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="16"/>
-    </row>
-    <row r="39" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="17"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="18"/>
+      <c r="B22" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="15">
+        <f t="shared" si="0"/>
+        <v>1499.9999999999995</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="15">
+        <f t="shared" ref="E22:E24" si="1">(C22-C21)/(C8-C6)</f>
+        <v>-32000.000000000011</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="15">
+        <f>(E22-E21)/(C8-C5)</f>
+        <v>60357.142857142877</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="15">
+        <f>(G22-G21)/(C8-C4)</f>
+        <v>697380.95238095266</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="15">
+        <f t="shared" si="0"/>
+        <v>2800.0000000000005</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="15">
+        <f t="shared" si="1"/>
+        <v>13000.000000000009</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="15">
+        <f>(E23-E22)/(C9-C6)</f>
+        <v>300000.00000000017</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="15">
+        <f>(G23-G22)/(C9-C5)</f>
+        <v>-958571.42857142922</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="15">
+        <f t="shared" si="0"/>
+        <v>1900.0000000000005</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="15">
+        <f t="shared" si="1"/>
+        <v>-9000.0000000000018</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="15">
+        <f>(E24-E23)/(C10-C7)</f>
+        <v>-146666.66666666674</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="15">
+        <f>(G24-G23)/(C10-C6)</f>
+        <v>-2233333.3333333349</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.DSMT4" shapeId="2049" r:id="rId3">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.DSMT4" shapeId="2049" r:id="rId3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.DSMT4" shapeId="2050" r:id="rId5">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.DSMT4" shapeId="2050" r:id="rId5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.DSMT4" shapeId="2051" r:id="rId7">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>200025</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>666750</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.DSMT4" shapeId="2051" r:id="rId7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.DSMT4" shapeId="2052" r:id="rId9">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>200025</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.DSMT4" shapeId="2052" r:id="rId9"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </oleObjects>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se modifican las tablas de diferencias divididas y se agregan al informe
</commit_message>
<xml_diff>
--- a/Parcial-Ejercicio-Regresion.xlsx
+++ b/Parcial-Ejercicio-Regresion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicaucaeduco-my.sharepoint.com/personal/juanoa_unicauca_edu_co/Documents/UNIVERSIDAD/Semestre2021.1/Analisis Numerico/Parcial-2-2021-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="599" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{88FEB871-F202-47FE-9FCC-5B1A14EFA38C}"/>
+  <xr:revisionPtr revIDLastSave="784" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{78E87767-3BD2-4757-9A95-4F9CCCFD6722}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -129,6 +129,27 @@
   <si>
     <t>F(X2,X3,X4,X5,X6)</t>
   </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>x-xi</t>
+  </si>
+  <si>
+    <t>interpolar x=</t>
+  </si>
+  <si>
+    <t>f(0,08)</t>
+  </si>
 </sst>
 </file>
 
@@ -143,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +201,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF68D000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -298,7 +337,48 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -316,10 +396,164 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -328,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -364,6 +598,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -373,10 +610,38 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -387,6 +652,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF6600"/>
+      <color rgb="FFCC99FF"/>
+      <color rgb="FF68D000"/>
       <color rgb="FF45F5A1"/>
     </mruColors>
   </colors>
@@ -1825,7 +2093,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.1</c:v>
@@ -1852,25 +2120,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1170</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1190</c:v>
+                  <c:v>1.1318324</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1255</c:v>
+                  <c:v>1.2297984</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1490</c:v>
+                  <c:v>1.2978518999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1565</c:v>
+                  <c:v>1.3401715999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1705</c:v>
+                  <c:v>1.3610329999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1800</c:v>
+                  <c:v>1.3646898000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4879,7 +5147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H64"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -5188,8 +5456,8 @@
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" s="2"/>
@@ -5230,25 +5498,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75BD078-DD7C-4543-9D69-F110EEC51D30}">
-  <dimension ref="B3:M32"/>
+  <dimension ref="B3:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5260,7 +5530,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="6">
-        <v>1170</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -5268,10 +5538,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="6">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="D5" s="6">
-        <v>1190</v>
+        <v>1.1318324</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -5282,7 +5552,7 @@
         <v>0.1</v>
       </c>
       <c r="D6" s="6">
-        <v>1255</v>
+        <v>1.2297984</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -5293,7 +5563,7 @@
         <v>0.15</v>
       </c>
       <c r="D7" s="6">
-        <v>1490</v>
+        <v>1.2978518999999999</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -5304,7 +5574,7 @@
         <v>0.2</v>
       </c>
       <c r="D8" s="6">
-        <v>1565</v>
+        <v>1.3401715999999999</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -5315,7 +5585,7 @@
         <v>0.25</v>
       </c>
       <c r="D9" s="6">
-        <v>1705</v>
+        <v>1.3610329999999999</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -5326,7 +5596,7 @@
         <v>0.3</v>
       </c>
       <c r="D10" s="6">
-        <v>1800</v>
+        <v>1.3646898000000001</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -5337,197 +5607,409 @@
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="18" t="s">
+    <row r="18" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19" t="s">
+      <c r="G19" s="35"/>
+      <c r="H19" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19" t="s">
+      <c r="I19" s="20"/>
+      <c r="J19" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19" t="s">
+      <c r="K19" s="20"/>
+      <c r="L19" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="20"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="M19" s="20"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F20" s="12"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="13"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="15">
+      <c r="G21" s="30">
         <f>(D5-D4)/(C5-C4)</f>
-        <v>40</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="14" t="s">
+        <v>2.6366479999999992</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="15">
+        <f>(G22-G21)/(C6-C4)</f>
+        <v>-6.7732799999999926</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="15">
+        <f>(I22-I21)/(C7-C4)</f>
+        <v>5.2718666666666181</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M21" s="15">
+        <f>(K22-K21)/(C8-C4)</f>
+        <v>1.4986666666665327</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F22" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="15">
+      <c r="G22" s="30">
         <f>(D6-D5)/(C6-C5)</f>
-        <v>-162.5</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="15">
-        <f>(C20-C19)/(C6-C4)</f>
-        <v>-2025</v>
-      </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
+        <v>1.95932</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="15">
+        <f>(G23-G22)/(C7-C5)</f>
+        <v>-5.9824999999999999</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="22">
+        <f>(I23-I22)/(C8-C5)</f>
+        <v>5.5715999999999246</v>
+      </c>
+      <c r="L22" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="M22" s="22">
+        <f>(K23-K22)/(C9-C5)</f>
+        <v>0.64533333333469667</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F23" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="15">
-        <f t="shared" ref="C21:C24" si="0">(D7-D6)/(C7-C6)</f>
-        <v>4700.0000000000009</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="15">
-        <f>(C21-C20)/(C7-C5)</f>
-        <v>-13892.857142857147</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="15">
-        <f>(E21-E20)/(C7-C4)</f>
-        <v>-79119.047619047647</v>
-      </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
+      <c r="G23" s="30">
+        <f>(D7-D6)/(C7-C6)</f>
+        <v>1.36107</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="15">
+        <f>(G24-G23)/(C8-C6)</f>
+        <v>-5.1467600000000111</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="15">
+        <f>(I24-I23)/(C9-C6)</f>
+        <v>5.7006666666668639</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M23" s="15">
+        <f>(K24-K23)/(C10-C6)</f>
+        <v>-0.14533333333434761</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F24" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="15">
+      <c r="G24" s="30">
+        <f>(D8-D7)/(C8-C7)</f>
+        <v>0.84639399999999887</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="15">
+        <f>(G25-G24)/(C9-C7)</f>
+        <v>-4.2916599999999816</v>
+      </c>
+      <c r="J24" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="32">
+        <f>(I25-I24)/(C10-C7)</f>
+        <v>5.6715999999999944</v>
+      </c>
+      <c r="L24" s="14"/>
+      <c r="M24" s="15"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="30">
+        <f>(D9-D8)/(C9-C8)</f>
+        <v>0.41722800000000071</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="15">
+        <f>(G26-G25)/(C10-C8)</f>
+        <v>-3.4409199999999824</v>
+      </c>
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="34"/>
+    </row>
+    <row r="26" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="28">
+        <f>(D10-D9)/(C10-C9)</f>
+        <v>7.3136000000002546E-2</v>
+      </c>
+      <c r="H26" s="16"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="23"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f>$C$27-C30</f>
+        <v>0.08</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="F30" s="40">
+        <v>1</v>
+      </c>
+      <c r="G30" s="40">
+        <v>2.6366480000000001</v>
+      </c>
+      <c r="H30" s="40">
+        <v>-6.7732799999999997</v>
+      </c>
+      <c r="I30" s="40">
+        <v>5.2718666699999996</v>
+      </c>
+      <c r="K30">
+        <f>F30+G30*B30+H30*B30*B31+I30*B30*B31*B32</f>
+        <v>1.1944229183998401</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f t="shared" ref="B31:B33" si="0">$C$27-C31</f>
+        <v>0.03</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="D31" s="6">
+        <v>1.1318324</v>
+      </c>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32">
         <f t="shared" si="0"/>
-        <v>1499.9999999999995</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="15">
-        <f t="shared" ref="E22:E24" si="1">(C22-C21)/(C8-C6)</f>
-        <v>-32000.000000000011</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="15">
-        <f>(E22-E21)/(C8-C5)</f>
-        <v>60357.142857142877</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="15">
-        <f>(G22-G21)/(C8-C4)</f>
-        <v>697380.95238095266</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="15">
-        <f t="shared" si="0"/>
-        <v>2800.0000000000005</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="15">
-        <f t="shared" si="1"/>
-        <v>13000.000000000009</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" s="15">
-        <f>(E23-E22)/(C9-C6)</f>
-        <v>300000.00000000017</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I23" s="15">
-        <f>(G23-G22)/(C9-C5)</f>
-        <v>-958571.42857142922</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="15">
-        <f t="shared" si="0"/>
-        <v>1900.0000000000005</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="15">
-        <f t="shared" si="1"/>
-        <v>-9000.0000000000018</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="15">
-        <f>(E24-E23)/(C10-C7)</f>
-        <v>-146666.66666666674</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" s="15">
-        <f>(G24-G23)/(C10-C6)</f>
-        <v>-2233333.3333333349</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>-2.0000000000000004E-2</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D32" s="6">
+        <v>1.2297984</v>
+      </c>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
     </row>
+    <row r="33" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1.2978518999999999</v>
+      </c>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+    </row>
+    <row r="35" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="I36" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K36" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f>$C$27-C37</f>
+        <v>0.03</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1.1318324</v>
+      </c>
+      <c r="F37" s="26">
+        <v>1.1318324</v>
+      </c>
+      <c r="G37" s="26">
+        <v>1.95932</v>
+      </c>
+      <c r="H37" s="26">
+        <v>-5.9824999999999999</v>
+      </c>
+      <c r="I37" s="26">
+        <v>5.5716000000000001</v>
+      </c>
+      <c r="K37">
+        <f>F37+G37*B37+H37*B37*B38+I37*B37*B38*B39</f>
+        <v>1.1944355071999999</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f>$C$27-C38</f>
+        <v>-2.0000000000000004E-2</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1.2297984</v>
+      </c>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f t="shared" ref="B38:B39" si="1">$C$27-C39</f>
+        <v>-6.9999999999999993E-2</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1.2978518999999999</v>
+      </c>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+    </row>
+    <row r="40" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1.3401715999999999</v>
+      </c>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>